<commit_message>
Full rerun, not sure why I have new features :(
</commit_message>
<xml_diff>
--- a/untargeted/best_labeled_anno.xlsx
+++ b/untargeted/best_labeled_anno.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Documents\PARAGON\untargeted\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\Will\PARAGON\untargeted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BDFC65-9723-423B-9A35-F6FD05A87700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="best_labeled_anno.xlsx" sheetId="1" r:id="rId1"/>
@@ -727,7 +726,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -1538,22 +1537,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="128" workbookViewId="0">
-      <selection activeCell="A68" sqref="A65:A68"/>
+    <sheetView tabSelected="1" zoomScale="128" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="11.28515625" style="4" customWidth="1"/>
     <col min="5" max="5" width="22" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1585,7 +1584,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1615,7 +1614,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1639,7 +1638,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1669,7 +1668,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1699,7 +1698,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1726,7 +1725,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1756,7 +1755,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1780,7 +1779,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1804,7 +1803,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1828,7 +1827,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1852,7 +1851,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1879,7 +1878,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1904,7 +1903,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1931,7 +1930,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1958,7 +1957,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1986,7 +1985,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -2013,7 +2012,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -2038,7 +2037,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -2065,7 +2064,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -2092,7 +2091,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -2117,7 +2116,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -2150,7 +2149,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -2174,7 +2173,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -2201,7 +2200,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -2228,7 +2227,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -2252,7 +2251,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -2276,7 +2275,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -2300,7 +2299,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -2324,7 +2323,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -2348,7 +2347,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -2375,7 +2374,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -2402,7 +2401,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -2457,7 +2456,7 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -2485,7 +2484,7 @@
       </c>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -2513,7 +2512,7 @@
       </c>
       <c r="N36" s="2"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -2540,7 +2539,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -2567,7 +2566,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>57</v>
       </c>
@@ -2597,7 +2596,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -2627,7 +2626,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>59</v>
       </c>
@@ -2654,7 +2653,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>60</v>
       </c>
@@ -2681,7 +2680,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>61</v>
       </c>
@@ -2708,7 +2707,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>62</v>
       </c>
@@ -2735,7 +2734,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>63</v>
       </c>
@@ -2759,7 +2758,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>65</v>
       </c>
@@ -2783,7 +2782,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>66</v>
       </c>
@@ -2807,7 +2806,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>68</v>
       </c>
@@ -2831,7 +2830,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>70</v>
       </c>
@@ -2858,7 +2857,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>71</v>
       </c>
@@ -2885,7 +2884,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>72</v>
       </c>
@@ -2912,7 +2911,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>73</v>
       </c>
@@ -2939,7 +2938,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>74</v>
       </c>
@@ -2963,7 +2962,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>76</v>
       </c>
@@ -2987,7 +2986,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>78</v>
       </c>
@@ -3011,7 +3010,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>79</v>
       </c>
@@ -3035,7 +3034,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>80</v>
       </c>
@@ -3059,7 +3058,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>81</v>
       </c>
@@ -3083,7 +3082,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>82</v>
       </c>
@@ -3113,7 +3112,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>83</v>
       </c>
@@ -3137,7 +3136,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>85</v>
       </c>
@@ -3164,7 +3163,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>86</v>
       </c>
@@ -3188,7 +3187,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>87</v>
       </c>
@@ -3221,7 +3220,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>88</v>
       </c>
@@ -3251,7 +3250,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>89</v>
       </c>
@@ -3284,7 +3283,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>90</v>
       </c>
@@ -3309,7 +3308,7 @@
       </c>
       <c r="M66" s="4"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>91</v>
       </c>
@@ -3339,7 +3338,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>92</v>
       </c>
@@ -3372,7 +3371,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>93</v>
       </c>
@@ -3396,7 +3395,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>94</v>
       </c>
@@ -3423,7 +3422,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>95</v>
       </c>
@@ -3450,7 +3449,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>96</v>
       </c>
@@ -3477,7 +3476,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>97</v>
       </c>
@@ -3504,7 +3503,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>98</v>
       </c>
@@ -3528,7 +3527,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>100</v>
       </c>
@@ -3552,7 +3551,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>101</v>
       </c>
@@ -3576,7 +3575,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>102</v>
       </c>
@@ -3600,7 +3599,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>103</v>
       </c>
@@ -3624,7 +3623,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>104</v>
       </c>
@@ -3654,7 +3653,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>105</v>
       </c>
@@ -3681,7 +3680,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>106</v>
       </c>
@@ -3708,7 +3707,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K84" t="s">
         <v>226</v>
       </c>
@@ -3717,7 +3716,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K85" t="s">
         <v>232</v>
       </c>
@@ -3726,7 +3725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K86" t="s">
         <v>227</v>
       </c>
@@ -3735,7 +3734,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K87" t="s">
         <v>225</v>
       </c>
@@ -3744,7 +3743,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K88" t="s">
         <v>229</v>
       </c>

</xml_diff>